<commit_message>
update vonB param and do some reruns
</commit_message>
<xml_diff>
--- a/input/generate_OMs.xlsx
+++ b/input/generate_OMs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27CA4BD-4386-DD43-85B3-036780A96D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09D66BB-670C-B841-84A6-1FDA37C90F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{300BEDC4-A2BE-AF49-9D01-6F98FB1D297A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{300BEDC4-A2BE-AF49-9D01-6F98FB1D297A}"/>
   </bookViews>
   <sheets>
     <sheet name="OM_Exp1" sheetId="1" r:id="rId1"/>
@@ -90,19 +90,19 @@
     <t>SexRatio_NoGrwthDiff (F60, M40)</t>
   </si>
   <si>
-    <t>Growth_M (10,0)</t>
-  </si>
-  <si>
-    <t>Growth_M (0,10)</t>
-  </si>
-  <si>
-    <t>Growth_M (10,10)</t>
-  </si>
-  <si>
-    <t>Growth_M (10,30)</t>
-  </si>
-  <si>
-    <t>Growth_M (30,10)</t>
+    <t>Growth_M (15,0)</t>
+  </si>
+  <si>
+    <t>Growth_M (0,15)</t>
+  </si>
+  <si>
+    <t>Growth_M (15,15)</t>
+  </si>
+  <si>
+    <t>Growth_M (15,30)</t>
+  </si>
+  <si>
+    <t>Growth_M (30,15)</t>
   </si>
 </sst>
 </file>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D8BB4C-3775-0945-9C13-0D6239EF8F83}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,7 +518,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -532,7 +532,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -540,10 +540,10 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="C5">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -562,7 +562,7 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="C7">
         <v>0.7</v>
@@ -576,7 +576,7 @@
         <v>0.7</v>
       </c>
       <c r="C8">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
     </row>
   </sheetData>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5C767B-2F74-2747-8052-199BF23D4AB8}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,10 +622,10 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="D2">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -636,10 +636,10 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="D3">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -650,10 +650,10 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="D4">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -664,10 +664,10 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="D5">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="D7">
         <v>1</v>

</xml_diff>